<commit_message>
on local on 29-06-2018 after question bank
</commit_message>
<xml_diff>
--- a/public/Download Question Bank Excel File.xlsx
+++ b/public/Download Question Bank Excel File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">question</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">right answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max</t>
   </si>
   <si>
     <t xml:space="preserve">question_type</t>
@@ -143,16 +149,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.2959183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -182,6 +191,12 @@
       </c>
       <c r="I1" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>